<commit_message>
add spring data jpa and h2 repositories
</commit_message>
<xml_diff>
--- a/src/main/resources/gantt/testing.xlsx
+++ b/src/main/resources/gantt/testing.xlsx
@@ -76,64 +76,64 @@
     <t>00с65гл+ВОсн130706</t>
   </si>
   <si>
-    <t>2019/04/13 19:51:19</t>
+    <t>2019/04/21 23:34:47</t>
   </si>
   <si>
     <t>0:20</t>
   </si>
   <si>
-    <t>2019/04/13 20:11:19</t>
+    <t>2019/04/21 23:54:47</t>
   </si>
   <si>
-    <t>2019/04/13 20:31:19</t>
+    <t>2019/04/22 00:14:47</t>
   </si>
   <si>
     <t>00с65гл+ВОсн261005</t>
   </si>
   <si>
-    <t>2019/04/13 20:51:19</t>
+    <t>2019/04/22 00:34:47</t>
   </si>
   <si>
-    <t>2019/04/13 21:11:19</t>
+    <t>2019/04/22 00:54:47</t>
   </si>
   <si>
     <t>08с6гл+во-у110701</t>
   </si>
   <si>
-    <t>2019/04/13 21:31:19</t>
+    <t>2019/04/22 01:14:47</t>
   </si>
   <si>
-    <t>2019/04/13 21:51:19</t>
+    <t>2019/04/22 01:34:47</t>
   </si>
   <si>
     <t>00с65гл+ВОсн191862</t>
   </si>
   <si>
-    <t>2019/04/13 22:11:19</t>
+    <t>2019/04/22 01:54:47</t>
   </si>
   <si>
-    <t>2019/04/13 22:31:19</t>
+    <t>2019/04/22 02:14:47</t>
   </si>
   <si>
     <t>0:15</t>
   </si>
   <si>
-    <t>2019/04/13 20:06:20</t>
+    <t>2019/04/21 23:49:48</t>
   </si>
   <si>
-    <t>2019/04/13 20:21:21</t>
+    <t>2019/04/22 00:04:49</t>
   </si>
   <si>
-    <t>2019/04/13 20:36:22</t>
+    <t>2019/04/22 00:19:50</t>
   </si>
   <si>
-    <t>2019/04/13 20:51:23</t>
+    <t>2019/04/22 00:34:52</t>
   </si>
   <si>
-    <t>2019/04/13 20:06:21</t>
+    <t>2019/04/21 23:49:49</t>
   </si>
   <si>
-    <t>2019/04/13 20:21:24</t>
+    <t>2019/04/22 00:04:52</t>
   </si>
   <si>
     <t>0:0</t>
@@ -142,10 +142,10 @@
     <t>7:435</t>
   </si>
   <si>
-    <t>2019/04/14 03:06:19</t>
+    <t>2019/04/22 06:49:47</t>
   </si>
   <si>
-    <t>2019/04/14 10:21:19</t>
+    <t>2019/04/22 14:04:47</t>
   </si>
 </sst>
 </file>

</xml_diff>